<commit_message>
dwellscanning eyetrack updated with new figures
</commit_message>
<xml_diff>
--- a/DwellScanningEyeTrack/img_training/Week10/map7.xlsx
+++ b/DwellScanningEyeTrack/img_training/Week10/map7.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\עמית 1 נוב 2013\פוסט\collaborations GCMRT\DP studies - NIH\Training task\Final - mixed blocks\Block 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\עמית 1 נוב 2013\פוסט\collaborations GCMRT\DP studies - NIH\Training task\Take 2\Final - mixed blocks\Block 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -90,10 +90,10 @@
     <t>block 7 matrix 1.bmp</t>
   </si>
   <si>
+    <t>DI</t>
+  </si>
+  <si>
     <t>NE</t>
-  </si>
-  <si>
-    <t>DI</t>
   </si>
   <si>
     <t>block 7 matrix 2.bmp</t>
@@ -1006,19 +1006,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="21" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="13" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1103,13 +1100,13 @@
         <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
@@ -1124,7 +1121,7 @@
         <v>23</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
         <v>23</v>
@@ -1136,7 +1133,7 @@
         <v>24</v>
       </c>
       <c r="R2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>24</v>
@@ -1145,7 +1142,7 @@
         <v>23</v>
       </c>
       <c r="U2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1168,10 +1165,10 @@
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>
@@ -1183,22 +1180,22 @@
         <v>24</v>
       </c>
       <c r="M3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S3" t="s">
         <v>24</v>
@@ -1224,22 +1221,22 @@
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -1254,22 +1251,22 @@
         <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q4" t="s">
         <v>24</v>
       </c>
       <c r="R4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T4" t="s">
         <v>24</v>
       </c>
       <c r="U4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1286,52 +1283,52 @@
         <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
         <v>24</v>
       </c>
       <c r="Q5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R5" t="s">
         <v>24</v>
       </c>
       <c r="S5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T5" t="s">
         <v>23</v>
       </c>
       <c r="U5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1357,7 +1354,7 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -1369,10 +1366,10 @@
         <v>24</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s">
         <v>23</v>
@@ -1381,16 +1378,16 @@
         <v>23</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S6" t="s">
         <v>24</v>
       </c>
       <c r="T6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U6" t="s">
         <v>24</v>
@@ -1410,22 +1407,22 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" t="s">
         <v>24</v>
@@ -1437,7 +1434,7 @@
         <v>23</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
         <v>23</v>
@@ -1452,10 +1449,10 @@
         <v>24</v>
       </c>
       <c r="T7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1472,7 +1469,7 @@
         <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
@@ -1484,16 +1481,16 @@
         <v>24</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N8" t="s">
         <v>24</v>
@@ -1511,13 +1508,13 @@
         <v>23</v>
       </c>
       <c r="S8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1540,10 +1537,10 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
@@ -1552,34 +1549,34 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
         <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
       </c>
       <c r="Q9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1596,19 +1593,19 @@
         <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K10" t="s">
         <v>23</v>
@@ -1617,10 +1614,10 @@
         <v>24</v>
       </c>
       <c r="M10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O10" t="s">
         <v>23</v>
@@ -1632,16 +1629,16 @@
         <v>24</v>
       </c>
       <c r="R10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T10" t="s">
         <v>23</v>
       </c>
       <c r="U10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1658,25 +1655,25 @@
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
         <v>24</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K11" t="s">
         <v>23</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M11" t="s">
         <v>24</v>
@@ -1688,16 +1685,16 @@
         <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R11" t="s">
         <v>23</v>
       </c>
       <c r="S11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T11" t="s">
         <v>23</v>
@@ -1720,10 +1717,10 @@
         <v>34</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
@@ -1738,16 +1735,16 @@
         <v>23</v>
       </c>
       <c r="L12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M12" t="s">
         <v>24</v>
       </c>
       <c r="N12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P12" t="s">
         <v>24</v>
@@ -1762,7 +1759,7 @@
         <v>24</v>
       </c>
       <c r="T12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U12" t="s">
         <v>23</v>
@@ -1794,13 +1791,13 @@
         <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M13" t="s">
         <v>24</v>
@@ -1815,19 +1812,19 @@
         <v>23</v>
       </c>
       <c r="Q13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1844,16 +1841,16 @@
         <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J14" t="s">
         <v>24</v>
@@ -1862,16 +1859,16 @@
         <v>24</v>
       </c>
       <c r="L14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P14" t="s">
         <v>23</v>
@@ -1883,13 +1880,13 @@
         <v>23</v>
       </c>
       <c r="S14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T14" t="s">
         <v>24</v>
       </c>
       <c r="U14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -1906,19 +1903,19 @@
         <v>37</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>24</v>
@@ -1933,10 +1930,10 @@
         <v>24</v>
       </c>
       <c r="O15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q15" t="s">
         <v>24</v>
@@ -1974,10 +1971,10 @@
         <v>23</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
         <v>24</v>
@@ -1986,22 +1983,22 @@
         <v>23</v>
       </c>
       <c r="L16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
       </c>
       <c r="Q16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R16" t="s">
         <v>23</v>
@@ -2013,7 +2010,7 @@
         <v>24</v>
       </c>
       <c r="U16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2030,16 +2027,16 @@
         <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H17" t="s">
         <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
         <v>24</v>
@@ -2048,7 +2045,7 @@
         <v>24</v>
       </c>
       <c r="L17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M17" t="s">
         <v>23</v>
@@ -2057,22 +2054,22 @@
         <v>23</v>
       </c>
       <c r="O17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P17" t="s">
         <v>23</v>
       </c>
       <c r="Q17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R17" t="s">
         <v>24</v>
       </c>
       <c r="S17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U17" t="s">
         <v>23</v>
@@ -2098,46 +2095,46 @@
         <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I18" t="s">
         <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" t="s">
         <v>24</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R18" t="s">
         <v>23</v>
       </c>
       <c r="S18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T18" t="s">
         <v>23</v>
       </c>
       <c r="U18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2163,10 +2160,10 @@
         <v>23</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K19" t="s">
         <v>24</v>
@@ -2178,7 +2175,7 @@
         <v>24</v>
       </c>
       <c r="N19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O19" t="s">
         <v>24</v>
@@ -2190,16 +2187,16 @@
         <v>23</v>
       </c>
       <c r="R19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T19" t="s">
         <v>24</v>
       </c>
       <c r="U19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2216,16 +2213,16 @@
         <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G20" t="s">
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
@@ -2237,10 +2234,10 @@
         <v>23</v>
       </c>
       <c r="M20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O20" t="s">
         <v>23</v>
@@ -2249,16 +2246,16 @@
         <v>24</v>
       </c>
       <c r="Q20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S20" t="s">
         <v>23</v>
       </c>
       <c r="T20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U20" t="s">
         <v>24</v>
@@ -2278,16 +2275,16 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
       </c>
       <c r="I21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J21" t="s">
         <v>24</v>
@@ -2296,22 +2293,22 @@
         <v>23</v>
       </c>
       <c r="L21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O21" t="s">
         <v>24</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R21" t="s">
         <v>23</v>
@@ -2320,10 +2317,10 @@
         <v>24</v>
       </c>
       <c r="T21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2340,28 +2337,28 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H22" t="s">
         <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
       <c r="M22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N22" t="s">
         <v>24</v>
@@ -2370,7 +2367,7 @@
         <v>24</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q22" t="s">
         <v>23</v>
@@ -2379,13 +2376,13 @@
         <v>23</v>
       </c>
       <c r="S22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2408,43 +2405,43 @@
         <v>23</v>
       </c>
       <c r="H23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O23" t="s">
         <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R23" t="s">
         <v>24</v>
       </c>
       <c r="S23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U23" t="s">
         <v>24</v>
@@ -2464,22 +2461,22 @@
         <v>46</v>
       </c>
       <c r="F24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H24" t="s">
         <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
       <c r="K24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L24" t="s">
         <v>24</v>
@@ -2491,7 +2488,7 @@
         <v>24</v>
       </c>
       <c r="O24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P24" t="s">
         <v>23</v>
@@ -2500,13 +2497,13 @@
         <v>23</v>
       </c>
       <c r="R24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="U24" t="s">
         <v>24</v>
@@ -2526,19 +2523,19 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G25" t="s">
         <v>23</v>
       </c>
       <c r="H25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K25" t="s">
         <v>23</v>
@@ -2547,10 +2544,10 @@
         <v>24</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O25" t="s">
         <v>23</v>
@@ -2559,7 +2556,7 @@
         <v>24</v>
       </c>
       <c r="Q25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R25" t="s">
         <v>24</v>
@@ -2571,7 +2568,7 @@
         <v>24</v>
       </c>
       <c r="U25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2588,7 +2585,7 @@
         <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" t="s">
         <v>23</v>
@@ -2597,25 +2594,25 @@
         <v>23</v>
       </c>
       <c r="I26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K26" t="s">
         <v>23</v>
       </c>
       <c r="L26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N26" t="s">
         <v>24</v>
       </c>
       <c r="O26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P26" t="s">
         <v>24</v>
@@ -2624,10 +2621,10 @@
         <v>24</v>
       </c>
       <c r="R26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T26" t="s">
         <v>23</v>
@@ -2650,7 +2647,7 @@
         <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
@@ -2671,28 +2668,28 @@
         <v>23</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q27" t="s">
         <v>23</v>
       </c>
       <c r="R27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U27" t="s">
         <v>24</v>
@@ -2712,25 +2709,25 @@
         <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" t="s">
         <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K28" t="s">
         <v>24</v>
       </c>
       <c r="L28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M28" t="s">
         <v>24</v>
@@ -2739,13 +2736,13 @@
         <v>23</v>
       </c>
       <c r="O28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P28" t="s">
         <v>23</v>
       </c>
       <c r="Q28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R28" t="s">
         <v>23</v>
@@ -2754,7 +2751,7 @@
         <v>23</v>
       </c>
       <c r="T28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U28" t="s">
         <v>24</v>
@@ -2774,7 +2771,7 @@
         <v>51</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G29" t="s">
         <v>24</v>
@@ -2783,7 +2780,7 @@
         <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J29" t="s">
         <v>23</v>
@@ -2792,7 +2789,7 @@
         <v>24</v>
       </c>
       <c r="L29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M29" t="s">
         <v>23</v>
@@ -2804,22 +2801,22 @@
         <v>23</v>
       </c>
       <c r="P29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R29" t="s">
         <v>24</v>
       </c>
       <c r="S29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="T29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2839,31 +2836,31 @@
         <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H30" t="s">
         <v>23</v>
       </c>
       <c r="I30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J30" t="s">
         <v>23</v>
       </c>
       <c r="K30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L30" t="s">
         <v>24</v>
       </c>
       <c r="M30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N30" t="s">
         <v>23</v>
       </c>
       <c r="O30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P30" t="s">
         <v>23</v>
@@ -2881,7 +2878,7 @@
         <v>23</v>
       </c>
       <c r="U30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2898,10 +2895,10 @@
         <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H31" t="s">
         <v>23</v>
@@ -2910,7 +2907,7 @@
         <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K31" t="s">
         <v>24</v>
@@ -2919,31 +2916,31 @@
         <v>23</v>
       </c>
       <c r="M31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N31" t="s">
         <v>23</v>
       </c>
       <c r="O31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q31" t="s">
         <v>24</v>
       </c>
       <c r="R31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>